<commit_message>
fixed problems with yellow and red
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottmcnally/Developer/Work AIB/Java Tools/SANHouseKeepingTool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BEA751-C1FE-864C-83AF-8B5AA4466975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047A1120-C9AB-754F-836A-1BB73F664C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{2DAFB9AF-8EF6-F44A-B2C5-175F605DEE79}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>PortName on FID 20</t>
   </si>
@@ -68,9 +68,6 @@
     <t>port 3</t>
   </si>
   <si>
-    <t>ALP_6520_DISK_1..72</t>
-  </si>
-  <si>
     <t>port 72</t>
   </si>
   <si>
@@ -78,6 +75,15 @@
   </si>
   <si>
     <t>ALP_X6_DISK_1.F_PORT.194.</t>
+  </si>
+  <si>
+    <t>ALP_X6_DISK_1.F_PORT.5.</t>
+  </si>
+  <si>
+    <t>ALP_X6_DISK_2.F_PORT.5.</t>
+  </si>
+  <si>
+    <t>ALP_6520_DISK_1..72.</t>
   </si>
 </sst>
 </file>
@@ -449,7 +455,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,16 +505,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -516,18 +522,27 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>